<commit_message>
removed crisis recovery page
</commit_message>
<xml_diff>
--- a/data/chicago_strategy_meeting_scores.xlsx
+++ b/data/chicago_strategy_meeting_scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jbecker\lgimapy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE17E52-3BB7-4665-91F0-C313BE0050B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E903243-D580-46AF-8C28-5E7F62DB57B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="5055" windowWidth="43200" windowHeight="23535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3 Months" sheetId="1" r:id="rId1"/>
@@ -511,11 +511,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X37" sqref="X37"/>
+      <selection pane="topRight" activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
     <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>43749</v>
       </c>
@@ -604,8 +604,11 @@
       <c r="AA1" s="1">
         <v>44628</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -687,8 +690,11 @@
       <c r="AA2">
         <v>-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -770,8 +776,11 @@
       <c r="AA3">
         <v>-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -853,8 +862,11 @@
       <c r="AA4">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -936,8 +948,11 @@
       <c r="AA5">
         <v>-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB5">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1019,8 +1034,11 @@
       <c r="AA6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1102,8 +1120,11 @@
       <c r="AA7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1185,8 +1206,11 @@
       <c r="AA8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1217,8 +1241,11 @@
       <c r="AA9">
         <v>-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -1273,8 +1300,11 @@
       <c r="AA10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1356,8 +1386,11 @@
       <c r="AA11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1439,8 +1472,11 @@
       <c r="AA12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1522,8 +1558,11 @@
       <c r="AA13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1605,8 +1644,11 @@
       <c r="AA14">
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1688,8 +1730,11 @@
       <c r="AA15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1771,8 +1816,11 @@
       <c r="AA16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB16">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1851,8 +1899,11 @@
       <c r="AA17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1931,8 +1982,11 @@
       <c r="AA18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2014,8 +2068,11 @@
       <c r="AA19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2095,7 +2152,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2174,8 +2231,11 @@
       <c r="AA21">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2257,8 +2317,11 @@
       <c r="AA22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2340,8 +2403,11 @@
       <c r="AA23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2423,8 +2489,11 @@
       <c r="AA24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2506,8 +2575,11 @@
       <c r="AA25">
         <v>-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2586,8 +2658,11 @@
       <c r="AA26">
         <v>-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2631,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2675,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2689,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -2738,11 +2813,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA27" sqref="AA27"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2827,7 @@
     <col min="26" max="26" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>43749</v>
       </c>
@@ -2831,8 +2906,11 @@
       <c r="AA1" s="1">
         <v>44628</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB1" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2914,8 +2992,11 @@
       <c r="AA2">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2997,8 +3078,11 @@
       <c r="AA3">
         <v>-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3080,8 +3164,11 @@
       <c r="AA4">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3163,8 +3250,11 @@
       <c r="AA5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3246,8 +3336,11 @@
       <c r="AA6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3329,8 +3422,11 @@
       <c r="AA7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3412,8 +3508,11 @@
       <c r="AA8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -3444,8 +3543,11 @@
       <c r="AA9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB9">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -3500,8 +3602,11 @@
       <c r="AA10">
         <v>-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3583,8 +3688,11 @@
       <c r="AA11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3666,8 +3774,11 @@
       <c r="AA12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3749,8 +3860,11 @@
       <c r="AA13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3832,8 +3946,11 @@
       <c r="AA14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3915,8 +4032,11 @@
       <c r="AA15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3998,8 +4118,11 @@
       <c r="AA16">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB16">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -4078,8 +4201,11 @@
       <c r="AA17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -4158,8 +4284,11 @@
       <c r="AA18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -4241,8 +4370,11 @@
       <c r="AA19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -4322,7 +4454,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -4401,8 +4533,11 @@
       <c r="AA21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -4484,8 +4619,11 @@
       <c r="AA22">
         <v>-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB22">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -4567,8 +4705,11 @@
       <c r="AA23">
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -4650,8 +4791,11 @@
       <c r="AA24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -4733,8 +4877,11 @@
       <c r="AA25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -4813,8 +4960,11 @@
       <c r="AA26">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB26">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4858,7 +5008,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -4899,7 +5049,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -4913,7 +5063,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -4962,11 +5112,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AX13"/>
+  <dimension ref="A1:AY13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ21" sqref="AZ21"/>
+      <selection pane="topRight" activeCell="AY14" sqref="AY14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,7 +5127,7 @@
     <col min="49" max="49" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>43070</v>
       </c>
@@ -5125,8 +5275,11 @@
       <c r="AX1" s="1">
         <v>44628</v>
       </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY1" s="1">
+        <v>44656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -5277,8 +5430,11 @@
       <c r="AX2">
         <v>-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -5429,8 +5585,11 @@
       <c r="AX3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY3">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -5581,8 +5740,11 @@
       <c r="AX4">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -5733,8 +5895,11 @@
       <c r="AX5">
         <v>-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY5">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -5885,8 +6050,11 @@
       <c r="AX6">
         <v>-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -6037,8 +6205,11 @@
       <c r="AX7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -6190,8 +6361,11 @@
       <c r="AX8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -6342,8 +6516,11 @@
       <c r="AX9">
         <v>-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -6416,8 +6593,11 @@
       <c r="AX10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -6508,8 +6688,11 @@
       <c r="AX11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -6600,8 +6783,11 @@
       <c r="AX12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -6655,6 +6841,9 @@
       </c>
       <c r="AX13">
         <v>0</v>
+      </c>
+      <c r="AY13">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>